<commit_message>
Updates time to boundary - functions2
</commit_message>
<xml_diff>
--- a/StatisticalAnalysis/TR_T1F_T2F_T3.xlsx
+++ b/StatisticalAnalysis/TR_T1F_T2F_T3.xlsx
@@ -558,7 +558,7 @@
         <v>1</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S2">
         <v>0</v>
@@ -567,7 +567,7 @@
         <v>1</v>
       </c>
       <c r="U2">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -818,13 +818,13 @@
         <v>0</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S6">
         <v>0</v>
       </c>
       <c r="T6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U6">
         <v>0</v>
@@ -883,7 +883,7 @@
         <v>1</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S7">
         <v>1</v>
@@ -892,7 +892,7 @@
         <v>1</v>
       </c>
       <c r="U7">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -948,7 +948,7 @@
         <v>1</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S8">
         <v>0</v>
@@ -957,7 +957,7 @@
         <v>1</v>
       </c>
       <c r="U8">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -1013,13 +1013,13 @@
         <v>0</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S9">
         <v>0</v>
       </c>
       <c r="T9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U9">
         <v>0</v>
@@ -1081,13 +1081,13 @@
         <v>0</v>
       </c>
       <c r="S10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T10">
         <v>1</v>
       </c>
       <c r="U10">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1143,16 +1143,16 @@
         <v>1</v>
       </c>
       <c r="R11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T11">
         <v>1</v>
       </c>
       <c r="U11">
-        <v>1</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -1208,7 +1208,7 @@
         <v>1</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S12">
         <v>1</v>
@@ -1217,7 +1217,7 @@
         <v>1</v>
       </c>
       <c r="U12">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -1338,7 +1338,7 @@
         <v>1</v>
       </c>
       <c r="R14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S14">
         <v>0</v>
@@ -1347,7 +1347,7 @@
         <v>1</v>
       </c>
       <c r="U14">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -1403,7 +1403,7 @@
         <v>1</v>
       </c>
       <c r="R15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S15">
         <v>0</v>
@@ -1412,7 +1412,7 @@
         <v>1</v>
       </c>
       <c r="U15">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -1468,7 +1468,7 @@
         <v>1</v>
       </c>
       <c r="R16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S16">
         <v>0</v>
@@ -1477,7 +1477,7 @@
         <v>1</v>
       </c>
       <c r="U16">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -1533,7 +1533,7 @@
         <v>1</v>
       </c>
       <c r="R17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S17">
         <v>1</v>
@@ -1542,7 +1542,7 @@
         <v>1</v>
       </c>
       <c r="U17">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:21">
@@ -1598,7 +1598,7 @@
         <v>1</v>
       </c>
       <c r="R18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S18">
         <v>1</v>
@@ -1607,7 +1607,7 @@
         <v>1</v>
       </c>
       <c r="U18">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -1660,19 +1660,19 @@
         <v>0.108</v>
       </c>
       <c r="Q19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R19">
         <v>0</v>
       </c>
       <c r="S19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U19">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -1790,19 +1790,19 @@
         <v>0</v>
       </c>
       <c r="Q21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S21">
         <v>0</v>
       </c>
       <c r="T21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U21">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:21">
@@ -1858,7 +1858,7 @@
         <v>1</v>
       </c>
       <c r="R22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S22">
         <v>1</v>
@@ -1867,7 +1867,7 @@
         <v>1</v>
       </c>
       <c r="U22">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:21">
@@ -1923,13 +1923,13 @@
         <v>0</v>
       </c>
       <c r="R23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S23">
         <v>0</v>
       </c>
       <c r="T23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U23">
         <v>0</v>
@@ -1988,13 +1988,13 @@
         <v>0</v>
       </c>
       <c r="R24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S24">
         <v>0</v>
       </c>
       <c r="T24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U24">
         <v>0</v>
@@ -2050,19 +2050,19 @@
         <v>0.09187082405345211</v>
       </c>
       <c r="Q25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R25">
         <v>0</v>
       </c>
       <c r="S25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U25">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:21">
@@ -2118,7 +2118,7 @@
         <v>1</v>
       </c>
       <c r="R26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S26">
         <v>1</v>
@@ -2127,7 +2127,7 @@
         <v>1</v>
       </c>
       <c r="U26">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:21">
@@ -2180,19 +2180,19 @@
         <v>0.09820627802690582</v>
       </c>
       <c r="Q27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U27">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:21">
@@ -2245,19 +2245,19 @@
         <v>0</v>
       </c>
       <c r="Q28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S28">
         <v>0</v>
       </c>
       <c r="T28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U28">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:21">
@@ -2313,13 +2313,13 @@
         <v>0</v>
       </c>
       <c r="R29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S29">
         <v>0</v>
       </c>
       <c r="T29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U29">
         <v>0</v>
@@ -2378,7 +2378,7 @@
         <v>1</v>
       </c>
       <c r="R30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S30">
         <v>1</v>
@@ -2387,7 +2387,7 @@
         <v>1</v>
       </c>
       <c r="U30">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:21">
@@ -2508,13 +2508,13 @@
         <v>0</v>
       </c>
       <c r="R32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S32">
         <v>0</v>
       </c>
       <c r="T32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U32">
         <v>0</v>
@@ -2570,19 +2570,19 @@
         <v>0.09534883720930232</v>
       </c>
       <c r="Q33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R33">
         <v>0</v>
       </c>
       <c r="S33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U33">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:21">
@@ -2641,10 +2641,10 @@
         <v>0</v>
       </c>
       <c r="S34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U34">
         <v>0</v>
@@ -2833,7 +2833,7 @@
         <v>1</v>
       </c>
       <c r="R37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S37">
         <v>0</v>
@@ -2842,7 +2842,7 @@
         <v>1</v>
       </c>
       <c r="U37">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:21">
@@ -3090,19 +3090,19 @@
         <v>0</v>
       </c>
       <c r="Q41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S41">
         <v>0</v>
       </c>
       <c r="T41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U41">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:21">
@@ -3158,7 +3158,7 @@
         <v>1</v>
       </c>
       <c r="R42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S42">
         <v>1</v>
@@ -3167,7 +3167,7 @@
         <v>1</v>
       </c>
       <c r="U42">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:21">
@@ -3486,13 +3486,13 @@
         <v>0</v>
       </c>
       <c r="S47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T47">
         <v>1</v>
       </c>
       <c r="U47">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:21">
@@ -3545,7 +3545,7 @@
         <v>0.25</v>
       </c>
       <c r="Q48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R48">
         <v>0</v>
@@ -3557,7 +3557,7 @@
         <v>1</v>
       </c>
       <c r="U48">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:21">
@@ -3610,19 +3610,19 @@
         <v>0.1021276595744681</v>
       </c>
       <c r="Q49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R49">
         <v>0</v>
       </c>
       <c r="S49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U49">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:21">
@@ -3678,7 +3678,7 @@
         <v>1</v>
       </c>
       <c r="R50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S50">
         <v>0</v>
@@ -3687,7 +3687,7 @@
         <v>1</v>
       </c>
       <c r="U50">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:21">
@@ -3743,13 +3743,13 @@
         <v>0</v>
       </c>
       <c r="R51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S51">
         <v>0</v>
       </c>
       <c r="T51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U51">
         <v>0</v>
@@ -3876,10 +3876,10 @@
         <v>0</v>
       </c>
       <c r="S53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U53">
         <v>0</v>
@@ -3941,10 +3941,10 @@
         <v>0</v>
       </c>
       <c r="S54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U54">
         <v>0</v>
@@ -4068,7 +4068,7 @@
         <v>1</v>
       </c>
       <c r="R56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S56">
         <v>0</v>
@@ -4077,7 +4077,7 @@
         <v>1</v>
       </c>
       <c r="U56">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:21">
@@ -4133,7 +4133,7 @@
         <v>1</v>
       </c>
       <c r="R57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S57">
         <v>0</v>
@@ -4142,7 +4142,7 @@
         <v>1</v>
       </c>
       <c r="U57">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:21">
@@ -4260,19 +4260,19 @@
         <v>0</v>
       </c>
       <c r="Q59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S59">
         <v>0</v>
       </c>
       <c r="T59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U59">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:21">
@@ -4328,7 +4328,7 @@
         <v>1</v>
       </c>
       <c r="R60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S60">
         <v>0</v>
@@ -4337,7 +4337,7 @@
         <v>1</v>
       </c>
       <c r="U60">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:21">
@@ -4393,7 +4393,7 @@
         <v>1</v>
       </c>
       <c r="R61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S61">
         <v>1</v>
@@ -4402,7 +4402,7 @@
         <v>1</v>
       </c>
       <c r="U61">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="62" spans="1:21">
@@ -4458,13 +4458,13 @@
         <v>0</v>
       </c>
       <c r="R62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S62">
         <v>0</v>
       </c>
       <c r="T62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U62">
         <v>0</v>
@@ -4523,13 +4523,13 @@
         <v>0</v>
       </c>
       <c r="R63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S63">
         <v>0</v>
       </c>
       <c r="T63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U63">
         <v>0</v>
@@ -4653,13 +4653,13 @@
         <v>0</v>
       </c>
       <c r="R65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S65">
         <v>0</v>
       </c>
       <c r="T65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U65">
         <v>0</v>
@@ -4718,7 +4718,7 @@
         <v>1</v>
       </c>
       <c r="R66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S66">
         <v>0</v>
@@ -4727,7 +4727,7 @@
         <v>1</v>
       </c>
       <c r="U66">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:21">
@@ -4780,19 +4780,19 @@
         <v>0</v>
       </c>
       <c r="Q67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S67">
         <v>0</v>
       </c>
       <c r="T67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U67">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:21">
@@ -4913,16 +4913,16 @@
         <v>0</v>
       </c>
       <c r="R69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U69">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="70" spans="1:21">
@@ -4978,7 +4978,7 @@
         <v>1</v>
       </c>
       <c r="R70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S70">
         <v>1</v>
@@ -4987,7 +4987,7 @@
         <v>1</v>
       </c>
       <c r="U70">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="71" spans="1:21">
@@ -5108,13 +5108,13 @@
         <v>0</v>
       </c>
       <c r="R72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S72">
         <v>0</v>
       </c>
       <c r="T72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U72">
         <v>0</v>
@@ -5170,19 +5170,19 @@
         <v>0</v>
       </c>
       <c r="Q73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S73">
         <v>0</v>
       </c>
       <c r="T73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U73">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:21">
@@ -5235,19 +5235,19 @@
         <v>0.108</v>
       </c>
       <c r="Q74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U74">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="75" spans="1:21">
@@ -5436,10 +5436,10 @@
         <v>0</v>
       </c>
       <c r="S77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U77">
         <v>0</v>
@@ -5563,7 +5563,7 @@
         <v>1</v>
       </c>
       <c r="R79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S79">
         <v>0</v>
@@ -5572,7 +5572,7 @@
         <v>1</v>
       </c>
       <c r="U79">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="80" spans="1:21">
@@ -5628,7 +5628,7 @@
         <v>1</v>
       </c>
       <c r="R80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S80">
         <v>0</v>
@@ -5637,7 +5637,7 @@
         <v>1</v>
       </c>
       <c r="U80">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="81" spans="1:21">
@@ -5690,19 +5690,19 @@
         <v>0.1169164882226981</v>
       </c>
       <c r="Q81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R81">
         <v>0</v>
       </c>
       <c r="S81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U81">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="82" spans="1:21">
@@ -5755,19 +5755,19 @@
         <v>0</v>
       </c>
       <c r="Q82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S82">
         <v>0</v>
       </c>
       <c r="T82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U82">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:21">
@@ -5823,13 +5823,13 @@
         <v>0</v>
       </c>
       <c r="R83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S83">
         <v>0</v>
       </c>
       <c r="T83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U83">
         <v>0</v>
@@ -5888,16 +5888,16 @@
         <v>1</v>
       </c>
       <c r="R84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T84">
         <v>1</v>
       </c>
       <c r="U84">
-        <v>1</v>
+        <v>123</v>
       </c>
     </row>
     <row r="85" spans="1:21">
@@ -5953,7 +5953,7 @@
         <v>1</v>
       </c>
       <c r="R85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S85">
         <v>0</v>
@@ -5962,7 +5962,7 @@
         <v>1</v>
       </c>
       <c r="U85">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="86" spans="1:21">
@@ -6018,13 +6018,13 @@
         <v>0</v>
       </c>
       <c r="R86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S86">
         <v>0</v>
       </c>
       <c r="T86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U86">
         <v>0</v>
@@ -6083,13 +6083,13 @@
         <v>0</v>
       </c>
       <c r="R87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S87">
         <v>0</v>
       </c>
       <c r="T87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U87">
         <v>0</v>
@@ -6148,7 +6148,7 @@
         <v>1</v>
       </c>
       <c r="R88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S88">
         <v>0</v>
@@ -6157,7 +6157,7 @@
         <v>1</v>
       </c>
       <c r="U88">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="89" spans="1:21">
@@ -6213,16 +6213,16 @@
         <v>1</v>
       </c>
       <c r="R89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T89">
         <v>1</v>
       </c>
       <c r="U89">
-        <v>1</v>
+        <v>123</v>
       </c>
     </row>
     <row r="90" spans="1:21">
@@ -6278,16 +6278,16 @@
         <v>1</v>
       </c>
       <c r="R90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T90">
         <v>1</v>
       </c>
       <c r="U90">
-        <v>1</v>
+        <v>123</v>
       </c>
     </row>
     <row r="91" spans="1:21">
@@ -6343,13 +6343,13 @@
         <v>0</v>
       </c>
       <c r="R91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S91">
         <v>0</v>
       </c>
       <c r="T91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U91">
         <v>0</v>
@@ -6408,16 +6408,16 @@
         <v>1</v>
       </c>
       <c r="R92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T92">
         <v>1</v>
       </c>
       <c r="U92">
-        <v>1</v>
+        <v>123</v>
       </c>
     </row>
     <row r="93" spans="1:21">
@@ -6473,7 +6473,7 @@
         <v>1</v>
       </c>
       <c r="R93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S93">
         <v>0</v>
@@ -6482,7 +6482,7 @@
         <v>1</v>
       </c>
       <c r="U93">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="94" spans="1:21">
@@ -6538,7 +6538,7 @@
         <v>1</v>
       </c>
       <c r="R94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S94">
         <v>0</v>
@@ -6547,7 +6547,7 @@
         <v>1</v>
       </c>
       <c r="U94">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="95" spans="1:21">
@@ -6603,13 +6603,13 @@
         <v>0</v>
       </c>
       <c r="R95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S95">
         <v>0</v>
       </c>
       <c r="T95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U95">
         <v>0</v>
@@ -6795,19 +6795,19 @@
         <v>0</v>
       </c>
       <c r="Q98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S98">
         <v>0</v>
       </c>
       <c r="T98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U98">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="99" spans="1:21">
@@ -6931,10 +6931,10 @@
         <v>0</v>
       </c>
       <c r="S100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U100">
         <v>0</v>
@@ -6993,13 +6993,13 @@
         <v>0</v>
       </c>
       <c r="R101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S101">
         <v>0</v>
       </c>
       <c r="T101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U101">
         <v>0</v>
@@ -7058,16 +7058,16 @@
         <v>0</v>
       </c>
       <c r="R102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U102">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="103" spans="1:21">
@@ -7185,19 +7185,19 @@
         <v>0.09820627802690582</v>
       </c>
       <c r="Q104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R104">
         <v>0</v>
       </c>
       <c r="S104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U104">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="105" spans="1:21">
@@ -7383,7 +7383,7 @@
         <v>1</v>
       </c>
       <c r="R107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S107">
         <v>1</v>
@@ -7392,7 +7392,7 @@
         <v>1</v>
       </c>
       <c r="U107">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="108" spans="1:21">
@@ -7448,7 +7448,7 @@
         <v>1</v>
       </c>
       <c r="R108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S108">
         <v>1</v>
@@ -7457,7 +7457,7 @@
         <v>1</v>
       </c>
       <c r="U108">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="109" spans="1:21">
@@ -7510,19 +7510,19 @@
         <v>0</v>
       </c>
       <c r="Q109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S109">
         <v>0</v>
       </c>
       <c r="T109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U109">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="110" spans="1:21">
@@ -7581,10 +7581,10 @@
         <v>0</v>
       </c>
       <c r="S110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U110">
         <v>0</v>
@@ -7705,19 +7705,19 @@
         <v>0.1045346062052506</v>
       </c>
       <c r="Q112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U112">
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="113" spans="1:21">
@@ -7773,13 +7773,13 @@
         <v>0</v>
       </c>
       <c r="R113">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S113">
         <v>0</v>
       </c>
       <c r="T113">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U113">
         <v>0</v>

</xml_diff>